<commit_message>
Late Scrum Update but might as well post it
</commit_message>
<xml_diff>
--- a/elsa/doc/Scrum_ELSA.xlsx
+++ b/elsa/doc/Scrum_ELSA.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amala\Desktop\Shared Folder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA80CAFD-D434-4F11-9007-9835DC1E8618}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E0CCC8B-7042-48ED-BF44-6F323FEBA702}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="173">
   <si>
     <t>Product Name:</t>
   </si>
@@ -462,9 +462,6 @@
     <t>Ensure ALL CODE is on GitHub by deadline!</t>
   </si>
   <si>
-    <t>--&gt; Add tasks to complete each feature for this sprint</t>
-  </si>
-  <si>
     <t>Finished in Sprint 1</t>
   </si>
   <si>
@@ -529,6 +526,36 @@
   </si>
   <si>
     <t>Finished in Sprint 3</t>
+  </si>
+  <si>
+    <t>Convert instert customer to 1 dialog</t>
+  </si>
+  <si>
+    <t>Entrey validation</t>
+  </si>
+  <si>
+    <t>Change to string to virtual</t>
+  </si>
+  <si>
+    <t>Change save to virtual</t>
+  </si>
+  <si>
+    <t>Create to_string for ram</t>
+  </si>
+  <si>
+    <t>Create save for ram</t>
+  </si>
+  <si>
+    <t>Convert order to one dialog</t>
+  </si>
+  <si>
+    <t>Convert Options to one dialog</t>
+  </si>
+  <si>
+    <t>Convert Desktop to one dialog</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 4</t>
   </si>
 </sst>
 </file>
@@ -832,7 +859,7 @@
     <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -953,10 +980,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -970,9 +997,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="18">
@@ -1222,10 +1246,10 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>11</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2374,7 +2398,7 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr sz="1300" b="0" strike="noStrike" spc="-1">
+              <a:rPr lang="en-US" sz="1300" b="0" strike="noStrike" spc="-1">
                 <a:latin typeface="Arial"/>
               </a:rPr>
               <a:t>Sprint Burn Chart</a:t>
@@ -2452,28 +2476,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2523,7 +2547,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Days</a:t>
@@ -2597,7 +2621,7 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr sz="900" b="0" strike="noStrike" spc="-1">
+                  <a:rPr lang="en-US" sz="900" b="0" strike="noStrike" spc="-1">
                     <a:latin typeface="Arial"/>
                   </a:rPr>
                   <a:t>Tasks</a:t>
@@ -3176,8 +3200,8 @@
   </sheetPr>
   <dimension ref="A1:AMK95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3219,7 +3243,7 @@
         <v>3</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C2" s="47"/>
       <c r="D2" s="47"/>
@@ -3265,7 +3289,7 @@
         <v>7</v>
       </c>
       <c r="B5" s="48" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="48"/>
       <c r="D5" s="48"/>
@@ -3273,7 +3297,7 @@
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
       <c r="H5" s="5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I5" s="5">
         <v>1001736019</v>
@@ -3459,11 +3483,11 @@
       </c>
       <c r="B16" s="2">
         <f>B15-C16</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C16" s="8">
         <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D16" s="8"/>
       <c r="E16" s="9"/>
@@ -3479,10 +3503,10 @@
       </c>
       <c r="B17" s="2">
         <f>B16-C17</f>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C17" s="8">
-        <f>COUNTIF(G$24:G$101,"Finished in Sprint 4")</f>
+        <f>COUNTIF(G$24:G$101,"Finished in Sprint 5")</f>
         <v>0</v>
       </c>
       <c r="D17" s="8"/>
@@ -3612,7 +3636,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H24" s="19" t="s">
         <v>31</v>
@@ -3643,7 +3667,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H25" s="19" t="s">
         <v>35</v>
@@ -3674,7 +3698,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H26" s="19" t="s">
         <v>31</v>
@@ -3705,7 +3729,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H27" s="19" t="s">
         <v>31</v>
@@ -3736,7 +3760,7 @@
         <v>2</v>
       </c>
       <c r="G28" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H28" s="19" t="s">
         <v>31</v>
@@ -3769,7 +3793,7 @@
         <v>2</v>
       </c>
       <c r="G29" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H29" s="19" t="s">
         <v>31</v>
@@ -3802,7 +3826,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H30" s="19" t="s">
         <v>31</v>
@@ -3835,7 +3859,7 @@
         <v>2</v>
       </c>
       <c r="G31" s="18" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H31" s="19" t="s">
         <v>57</v>
@@ -3866,7 +3890,7 @@
         <v>3</v>
       </c>
       <c r="G32" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H32" s="19" t="s">
         <v>61</v>
@@ -3899,7 +3923,7 @@
         <v>3</v>
       </c>
       <c r="G33" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H33" s="19" t="s">
         <v>61</v>
@@ -3932,7 +3956,7 @@
         <v>3</v>
       </c>
       <c r="G34" s="18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H34" s="19" t="s">
         <v>61</v>
@@ -3962,7 +3986,9 @@
         <v>21</v>
       </c>
       <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
+      <c r="G35" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="H35" s="19" t="s">
         <v>71</v>
       </c>
@@ -3989,7 +4015,9 @@
         <v>8</v>
       </c>
       <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
+      <c r="G36" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="H36" s="19" t="s">
         <v>31</v>
       </c>
@@ -4140,7 +4168,9 @@
         <v>21</v>
       </c>
       <c r="F43" s="18"/>
-      <c r="G43" s="18"/>
+      <c r="G43" s="18" t="s">
+        <v>172</v>
+      </c>
       <c r="H43" s="19" t="s">
         <v>31</v>
       </c>
@@ -4982,7 +5012,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5264,7 +5294,7 @@
         <v>122</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F17" s="43" t="s">
         <v>123</v>
@@ -5282,7 +5312,7 @@
         <v>124</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F18" s="43" t="s">
         <v>125</v>
@@ -5300,7 +5330,7 @@
         <v>126</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F19" s="43" t="s">
         <v>127</v>
@@ -5318,7 +5348,7 @@
         <v>128</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F20" s="43"/>
     </row>
@@ -5334,7 +5364,7 @@
         <v>129</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F21" s="43"/>
     </row>
@@ -5350,7 +5380,7 @@
         <v>130</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" s="43"/>
     </row>
@@ -5366,7 +5396,7 @@
         <v>131</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F23" s="43"/>
     </row>
@@ -5382,7 +5412,7 @@
         <v>132</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F24" s="43"/>
     </row>
@@ -5398,7 +5428,7 @@
         <v>133</v>
       </c>
       <c r="E25" s="42" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F25" s="43"/>
     </row>
@@ -5414,7 +5444,7 @@
         <v>134</v>
       </c>
       <c r="E26" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F26" s="43"/>
     </row>
@@ -5430,7 +5460,7 @@
         <v>135</v>
       </c>
       <c r="E27" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F27" s="43"/>
     </row>
@@ -5446,7 +5476,7 @@
         <v>136</v>
       </c>
       <c r="E28" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F28" s="43"/>
     </row>
@@ -5462,7 +5492,7 @@
         <v>137</v>
       </c>
       <c r="E29" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F29" s="43"/>
     </row>
@@ -5478,7 +5508,7 @@
         <v>138</v>
       </c>
       <c r="E30" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F30" s="43"/>
     </row>
@@ -5494,7 +5524,7 @@
         <v>139</v>
       </c>
       <c r="E31" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F31" s="43"/>
     </row>
@@ -5510,7 +5540,7 @@
         <v>140</v>
       </c>
       <c r="E32" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F32" s="43"/>
     </row>
@@ -6527,11 +6557,11 @@
         <v>44</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="45" t="s">
-        <v>148</v>
+      <c r="D17" s="44" t="s">
+        <v>147</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" s="43"/>
     </row>
@@ -6544,10 +6574,10 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F18" s="43"/>
     </row>
@@ -6560,10 +6590,10 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="41" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" s="43"/>
     </row>
@@ -6576,10 +6606,10 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="41" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F20" s="43"/>
     </row>
@@ -6592,10 +6622,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="41" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" s="43"/>
     </row>
@@ -6608,10 +6638,10 @@
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="41" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E22" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F22" s="43"/>
     </row>
@@ -6624,10 +6654,10 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="41" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="E23" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F23" s="43"/>
     </row>
@@ -6640,10 +6670,10 @@
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="41" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="E24" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F24" s="43"/>
     </row>
@@ -7740,11 +7770,11 @@
         <v>60</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="50" t="s">
-        <v>158</v>
+      <c r="D17" s="45" t="s">
+        <v>157</v>
       </c>
       <c r="E17" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F17" s="43"/>
     </row>
@@ -7757,10 +7787,10 @@
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="41" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F18" s="43"/>
     </row>
@@ -7773,10 +7803,10 @@
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="41" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="E19" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F19" s="43"/>
     </row>
@@ -7789,10 +7819,10 @@
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="41" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E20" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F20" s="43"/>
     </row>
@@ -7805,10 +7835,10 @@
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E21" s="42" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F21" s="43"/>
     </row>
@@ -8655,7 +8685,7 @@
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F100" sqref="F100"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -8762,7 +8792,7 @@
       </c>
       <c r="B7" s="30">
         <f>COUNTA(D17:D995)</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="30"/>
@@ -8777,7 +8807,7 @@
       </c>
       <c r="B8" s="30">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C8" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -8795,7 +8825,7 @@
       </c>
       <c r="B9" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C9" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -8813,7 +8843,7 @@
       </c>
       <c r="B10" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C10" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -8831,7 +8861,7 @@
       </c>
       <c r="B11" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C11" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -8849,7 +8879,7 @@
       </c>
       <c r="B12" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C12" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -8867,7 +8897,7 @@
       </c>
       <c r="B13" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C13" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -8885,11 +8915,11 @@
       </c>
       <c r="B14" s="30">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C14" s="30">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D14" s="30"/>
       <c r="E14" s="30"/>
@@ -8927,77 +8957,113 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>1</v>
       </c>
-      <c r="B17" s="40"/>
+      <c r="B17" s="40" t="s">
+        <v>74</v>
+      </c>
       <c r="C17" s="1"/>
-      <c r="D17" s="44" t="s">
-        <v>141</v>
-      </c>
-      <c r="E17" s="42"/>
-      <c r="F17" s="43" t="s">
-        <v>127</v>
-      </c>
+      <c r="D17" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>2</v>
       </c>
-      <c r="B18" s="40"/>
+      <c r="B18" s="40" t="s">
+        <v>74</v>
+      </c>
       <c r="C18" s="1"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="42"/>
+      <c r="D18" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="E18" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="40" t="s">
+        <v>70</v>
+      </c>
       <c r="C19" s="1"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="D19" s="41" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>4</v>
       </c>
-      <c r="B20" s="40"/>
+      <c r="B20" s="40" t="s">
+        <v>70</v>
+      </c>
       <c r="C20" s="1"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="42"/>
+      <c r="D20" s="41" t="s">
+        <v>166</v>
+      </c>
+      <c r="E20" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>5</v>
       </c>
-      <c r="B21" s="40"/>
+      <c r="B21" s="40" t="s">
+        <v>70</v>
+      </c>
       <c r="C21" s="1"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="42"/>
+      <c r="D21" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="E21" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>6</v>
       </c>
-      <c r="B22" s="40"/>
+      <c r="B22" s="40" t="s">
+        <v>70</v>
+      </c>
       <c r="C22" s="1"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="42"/>
+      <c r="D22" s="41" t="s">
+        <v>168</v>
+      </c>
+      <c r="E22" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>7</v>
       </c>
-      <c r="B23" s="40"/>
+      <c r="B23" s="40" t="s">
+        <v>83</v>
+      </c>
       <c r="C23" s="1"/>
-      <c r="D23" s="41"/>
+      <c r="D23" s="41" t="s">
+        <v>169</v>
+      </c>
       <c r="E23" s="42"/>
       <c r="F23" s="43"/>
     </row>
@@ -9005,19 +9071,29 @@
       <c r="A24" s="1">
         <v>8</v>
       </c>
-      <c r="B24" s="40"/>
+      <c r="B24" s="40" t="s">
+        <v>85</v>
+      </c>
       <c r="C24" s="1"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="42"/>
+      <c r="D24" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="E24" s="42" t="s">
+        <v>146</v>
+      </c>
       <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>9</v>
       </c>
-      <c r="B25" s="40"/>
+      <c r="B25" s="40" t="s">
+        <v>87</v>
+      </c>
       <c r="C25" s="1"/>
-      <c r="D25" s="41"/>
+      <c r="D25" s="41" t="s">
+        <v>171</v>
+      </c>
       <c r="E25" s="42"/>
       <c r="F25" s="43"/>
     </row>
@@ -9795,12 +9871,12 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">

</xml_diff>